<commit_message>
Change Codes to Prepare for Future Features (#241)
* Allow Roles Override

* Add Sidekick

* Fix Assign Self Bug (for GM and NotAssigned)

* Oh my gosh

* Oh my gosh p2

* OHHHHH MY GOSHHHHHH I FINALLY DID IT

* Remove Addons for Sidekick

* Optimize Codes

* Small Thing

* Update Jackal and Sidekick

* Try Fix Black Screen for Assign

* Fix Sidekick Cannot Win

* Add Lower Text for Jackal
</commit_message>
<xml_diff>
--- a/Assets/Roles ID.xlsx
+++ b/Assets/Roles ID.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Desktop\TONX\Assets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yuxia\Downloads\新建文件夹\TownOfNext\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B963AFC0-69A0-45E2-A7F9-309D560A9D5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBB22C37-4695-41F9-BBCE-B80EF118D171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="28920" windowHeight="15870" xr2:uid="{814C7422-745C-474F-A837-AE31BC6ADF7D}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13200" xr2:uid="{814C7422-745C-474F-A837-AE31BC6ADF7D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="115">
   <si>
     <t>Bodyguard</t>
   </si>
@@ -395,6 +393,10 @@
   </si>
   <si>
     <t>Hater</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sidekick</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -451,74 +453,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -535,10 +469,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="282C34"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="D8DEE9"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -829,18 +763,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B2AB7C1-B92C-442E-A860-0526D649E1E1}">
   <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.15" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.25" customWidth="1"/>
-    <col min="4" max="4" width="14.875" customWidth="1"/>
+    <col min="1" max="1" width="17.2109375" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
     <col min="7" max="7" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -866,7 +800,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -892,7 +826,7 @@
         <v>80000</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -918,7 +852,7 @@
         <v>80100</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -944,7 +878,7 @@
         <v>80200</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -970,7 +904,7 @@
         <v>80300</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -996,7 +930,7 @@
         <v>80400</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1022,7 +956,7 @@
         <v>80500</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1048,7 +982,7 @@
         <v>80600</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1074,7 +1008,7 @@
         <v>80700</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1100,7 +1034,7 @@
         <v>80800</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1126,7 +1060,7 @@
         <v>80900</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1152,7 +1086,7 @@
         <v>81000</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1178,7 +1112,7 @@
         <v>81100</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1204,7 +1138,7 @@
         <v>81200</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1230,7 +1164,7 @@
         <v>81300</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1256,7 +1190,7 @@
         <v>81400</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1269,6 +1203,12 @@
       <c r="E17">
         <v>2800</v>
       </c>
+      <c r="G17" t="s">
+        <v>114</v>
+      </c>
+      <c r="H17">
+        <v>51800</v>
+      </c>
       <c r="J17" t="s">
         <v>94</v>
       </c>
@@ -1276,7 +1216,7 @@
         <v>81500</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1296,7 +1236,7 @@
         <v>81600</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1316,7 +1256,7 @@
         <v>81700</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1336,7 +1276,7 @@
         <v>81800</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1356,7 +1296,7 @@
         <v>81900</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1376,7 +1316,7 @@
         <v>82000</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1396,7 +1336,7 @@
         <v>82100</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1410,7 +1350,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1424,7 +1364,7 @@
         <v>2600</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1438,7 +1378,7 @@
         <v>1900</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1452,7 +1392,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1466,7 +1406,7 @@
         <v>4700</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1480,7 +1420,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1494,7 +1434,7 @@
         <v>3700</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1508,7 +1448,7 @@
         <v>3000</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="D32" t="s">
         <v>62</v>
       </c>
@@ -1516,7 +1456,7 @@
         <v>1800</v>
       </c>
     </row>
-    <row r="33" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D33" t="s">
         <v>63</v>
       </c>
@@ -1524,7 +1464,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="34" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D34" t="s">
         <v>64</v>
       </c>
@@ -1532,7 +1472,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="35" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D35" t="s">
         <v>65</v>
       </c>
@@ -1540,7 +1480,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="36" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D36" t="s">
         <v>66</v>
       </c>
@@ -1548,7 +1488,7 @@
         <v>3900</v>
       </c>
     </row>
-    <row r="37" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D37" t="s">
         <v>67</v>
       </c>
@@ -1556,7 +1496,7 @@
         <v>2700</v>
       </c>
     </row>
-    <row r="38" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D38" t="s">
         <v>68</v>
       </c>
@@ -1564,7 +1504,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="39" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D39" t="s">
         <v>69</v>
       </c>
@@ -1572,7 +1512,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="40" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D40" t="s">
         <v>70</v>
       </c>
@@ -1580,7 +1520,7 @@
         <v>2100</v>
       </c>
     </row>
-    <row r="41" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="41" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D41" t="s">
         <v>71</v>
       </c>
@@ -1588,7 +1528,7 @@
         <v>4100</v>
       </c>
     </row>
-    <row r="43" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D43" t="s">
         <v>105</v>
       </c>
@@ -1596,7 +1536,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="44" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="44" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D44" t="s">
         <v>106</v>
       </c>
@@ -1604,7 +1544,7 @@
         <v>5100</v>
       </c>
     </row>
-    <row r="45" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="45" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D45" t="s">
         <v>107</v>
       </c>
@@ -1612,7 +1552,7 @@
         <v>5200</v>
       </c>
     </row>
-    <row r="46" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="46" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D46" t="s">
         <v>108</v>
       </c>
@@ -1620,7 +1560,7 @@
         <v>5300</v>
       </c>
     </row>
-    <row r="47" spans="4:5" x14ac:dyDescent="0.2">
+    <row r="47" spans="4:5" x14ac:dyDescent="0.35">
       <c r="D47" t="s">
         <v>109</v>
       </c>

</xml_diff>